<commit_message>
Added new SEO file; added references to audit and recommendations
</commit_message>
<xml_diff>
--- a/Template+SEO+analysis.xlsx
+++ b/Template+SEO+analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15c141d6a280b1ea/Desktop/gitProjects/repos/Tasya-MainHub/Project4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15c141d6a280b1ea/Desktop/gitProjects/repos/Project4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{F6B60CDE-FC3A-4FD4-9433-8DA2B1A8BD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AE21A4A3-075D-4229-8377-3DAF0ACDF5E5}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{F6B60CDE-FC3A-4FD4-9433-8DA2B1A8BD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5CEE454E-39C6-440E-87D8-4AC166F5DCB4}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1545" windowWidth="17490" windowHeight="8640" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
+    <workbookView xWindow="30615" yWindow="1935" windowWidth="10245" windowHeight="10920" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Explanation</t>
   </si>
@@ -125,27 +125,6 @@
     <t>Navigation is not consistent from one page to the other; navigation present on home page but not on contact page</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Contact page has a &lt;title&gt; element</t>
-  </si>
-  <si>
-    <t>Readability</t>
-  </si>
-  <si>
-    <t>Contact page uses legible font sizes</t>
-  </si>
-  <si>
-    <t>Buttons have an accessible name so it can be read by screen readers</t>
-  </si>
-  <si>
-    <t>Home page has a meta description for search results</t>
-  </si>
-  <si>
-    <t>Zoom hasn't been disabled on the page allowing users with low vision to zoom in as necessary</t>
-  </si>
-  <si>
     <t>Keyword Usage</t>
   </si>
   <si>
@@ -153,6 +132,54 @@
   </si>
   <si>
     <t>Image elements on second page do not have [alt] attributes and home page has non-descriptive [alt] attributes</t>
+  </si>
+  <si>
+    <t>Lighten text to add more contrast on dark background</t>
+  </si>
+  <si>
+    <t>Change name from page2 to Contact Me</t>
+  </si>
+  <si>
+    <t>Change from Default to en</t>
+  </si>
+  <si>
+    <t>update alt descriptions on images</t>
+  </si>
+  <si>
+    <t>add description to contact page</t>
+  </si>
+  <si>
+    <t>add a visible focus indicator for fous elements</t>
+  </si>
+  <si>
+    <t>space out links so they don't overlap; update margins</t>
+  </si>
+  <si>
+    <t>add a heading to Contact page</t>
+  </si>
+  <si>
+    <t>add "for" attribute in label element</t>
+  </si>
+  <si>
+    <t>change navigation so that the second page matchs first</t>
+  </si>
+  <si>
+    <t>delete white keywords; delete miscellaneous links</t>
+  </si>
+  <si>
+    <t>web.dv</t>
+  </si>
+  <si>
+    <t>w3.org</t>
+  </si>
+  <si>
+    <t>pcmag.com: https://www.pcmag.com/news/the-promises-and-pitfalls-of-black-hat-seo-practices; forbes.com https://www.forbes.com/sites/johnrampton/2015/07/29/25-black-hat-techniques-that-are-killing-your-seo/#efa216a64314</t>
+  </si>
+  <si>
+    <t>moz.com: Meta Description</t>
+  </si>
+  <si>
+    <t>moz.com: Mobile Optimization</t>
   </si>
 </sst>
 </file>
@@ -210,11 +237,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,266 +572,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21008D1C-867F-FF4D-8036-BD2682FF7900}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
-    <col min="4" max="4" width="43.375" customWidth="1"/>
-    <col min="5" max="5" width="43.875" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="1" max="1" width="27" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11" style="7"/>
+    <col min="4" max="4" width="43.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="43.875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
+      <c r="E12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added final file, updated SEO
</commit_message>
<xml_diff>
--- a/Template+SEO+analysis.xlsx
+++ b/Template+SEO+analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15c141d6a280b1ea/Desktop/gitProjects/repos/Project4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{F6B60CDE-FC3A-4FD4-9433-8DA2B1A8BD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5CEE454E-39C6-440E-87D8-4AC166F5DCB4}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{43566AC8-8947-6745-8A18-4766E7EB70FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{511920AB-877E-4E69-AEF9-234865CC0D56}"/>
   <bookViews>
-    <workbookView xWindow="30615" yWindow="1935" windowWidth="10245" windowHeight="10920" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{F4D0CAC2-2123-1946-879C-AB8072365C64}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Explanation</t>
   </si>
@@ -167,26 +167,44 @@
     <t>delete white keywords; delete miscellaneous links</t>
   </si>
   <si>
-    <t>web.dv</t>
-  </si>
-  <si>
-    <t>w3.org</t>
-  </si>
-  <si>
-    <t>pcmag.com: https://www.pcmag.com/news/the-promises-and-pitfalls-of-black-hat-seo-practices; forbes.com https://www.forbes.com/sites/johnrampton/2015/07/29/25-black-hat-techniques-that-are-killing-your-seo/#efa216a64314</t>
-  </si>
-  <si>
-    <t>moz.com: Meta Description</t>
-  </si>
-  <si>
-    <t>moz.com: Mobile Optimization</t>
+    <t>https://www.w3.org/WAI/WCAG21/quickref/#focus-visible</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/quickref/#consistent-navigation</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/quickref/#headings-and-labels</t>
+  </si>
+  <si>
+    <t>https://moz.com/learn/seo/mobile-optimization</t>
+  </si>
+  <si>
+    <t>https://moz.com/learn/seo/meta-description</t>
+  </si>
+  <si>
+    <t>https://web.dev/image-alt/</t>
+  </si>
+  <si>
+    <t>https://web.dev/label/</t>
+  </si>
+  <si>
+    <t>https://web.dev/color-contrast/</t>
+  </si>
+  <si>
+    <t>https://web.dev/link-text/</t>
+  </si>
+  <si>
+    <t>https://web.dev/html-has-lang/</t>
+  </si>
+  <si>
+    <t>pcmag.com: https://www.pcmag.com/news/the-promises-and-pitfalls-of-black-hat-seo-practices ; forbes.com https://www.forbes.com/sites/johnrampton/2015/07/29/25-black-hat-techniques-that-are-killing-your-seo/#efa216a64314</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +224,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,10 +260,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -258,8 +285,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21008D1C-867F-FF4D-8036-BD2682FF7900}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -624,8 +655,8 @@
       <c r="E2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>44</v>
+      <c r="F2" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -644,8 +675,8 @@
       <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
+      <c r="F3" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -664,8 +695,8 @@
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>44</v>
+      <c r="F4" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,8 +715,8 @@
       <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>44</v>
+      <c r="F5" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,11 +735,11 @@
       <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -724,8 +755,8 @@
       <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>45</v>
+      <c r="F7" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -744,11 +775,11 @@
       <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -764,8 +795,8 @@
       <c r="E9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>45</v>
+      <c r="F9" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,8 +815,8 @@
       <c r="E10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>44</v>
+      <c r="F10" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -804,7 +835,7 @@
       <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -825,11 +856,23 @@
         <v>43</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" location="focus-visible" xr:uid="{27585A30-1BB4-5741-A754-742141D8C203}"/>
+    <hyperlink ref="F11" r:id="rId2" location="consistent-navigation" xr:uid="{B89F0BE3-E49F-7849-95C4-13DF2C160505}"/>
+    <hyperlink ref="F9" r:id="rId3" location="headings-and-labels" xr:uid="{4E23D642-B1FB-6C4A-BA92-5060AC77AFB4}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{A16160A8-A7F6-5045-96A4-B6EDC83DDE52}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{939BAA93-9E73-3B41-B4EB-39A81923E9FC}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{F9282241-946B-6C40-91F1-A2EFE4901506}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{098DF229-1495-954D-9E1D-B080BE9B4EB9}"/>
+    <hyperlink ref="F2" r:id="rId8" xr:uid="{D90155F8-A1AB-E74B-A1D3-E6A1234590A5}"/>
+    <hyperlink ref="F3" r:id="rId9" xr:uid="{C48ADAA5-5362-A846-AD64-F66B326F317C}"/>
+    <hyperlink ref="F4" r:id="rId10" xr:uid="{41B29D97-6AE8-1347-9143-4E2008469824}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>